<commit_message>
re-ran lc data data
</commit_message>
<xml_diff>
--- a/raw_data/lc_data.xlsx
+++ b/raw_data/lc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Epigenomics/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joegunn/Desktop/Projects/active_projects/CPB_Phenotype/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BB2C18-42D1-BA4F-B376-83A530484E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE9E09F-5C67-924C-8D97-2073D8D49EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="329">
   <si>
     <t>assay</t>
   </si>
@@ -791,9 +791,6 @@
     <t>224</t>
   </si>
   <si>
-    <t>Missing</t>
-  </si>
-  <si>
     <t>225</t>
   </si>
   <si>
@@ -4259,7 +4256,7 @@
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
     </row>
-    <row r="47" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="3" t="s">
         <v>17</v>
       </c>
@@ -4323,7 +4320,7 @@
       <c r="Z47" s="2"/>
       <c r="AA47" s="2"/>
     </row>
-    <row r="48" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>17</v>
       </c>
@@ -4387,7 +4384,7 @@
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
     </row>
-    <row r="49" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
         <v>17</v>
       </c>
@@ -4451,7 +4448,7 @@
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
     </row>
-    <row r="50" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
         <v>17</v>
       </c>
@@ -15705,9 +15702,7 @@
       <c r="L225" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M225" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="M225" s="3"/>
       <c r="N225" s="3">
         <v>2</v>
       </c>
@@ -15763,7 +15758,7 @@
         <v>10</v>
       </c>
       <c r="K226" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L226" s="3" t="s">
         <v>22</v>
@@ -15826,7 +15821,7 @@
         <v>10</v>
       </c>
       <c r="K227" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L227" s="3" t="s">
         <v>22</v>
@@ -15889,7 +15884,7 @@
         <v>10</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L228" s="3" t="s">
         <v>22</v>
@@ -15952,7 +15947,7 @@
         <v>5</v>
       </c>
       <c r="K229" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L229" s="3" t="s">
         <v>22</v>
@@ -16015,7 +16010,7 @@
         <v>1</v>
       </c>
       <c r="K230" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L230" s="3" t="s">
         <v>22</v>
@@ -16078,7 +16073,7 @@
         <v>5</v>
       </c>
       <c r="K231" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L231" s="3" t="s">
         <v>22</v>
@@ -16141,7 +16136,7 @@
         <v>10</v>
       </c>
       <c r="K232" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L232" s="3" t="s">
         <v>22</v>
@@ -16204,7 +16199,7 @@
         <v>50</v>
       </c>
       <c r="K233" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L233" s="3" t="s">
         <v>22</v>
@@ -16267,7 +16262,7 @@
         <v>0</v>
       </c>
       <c r="K234" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="L234" s="3" t="s">
         <v>22</v>
@@ -16330,7 +16325,7 @@
         <v>10</v>
       </c>
       <c r="K235" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L235" s="3" t="s">
         <v>22</v>
@@ -16393,7 +16388,7 @@
         <v>5</v>
       </c>
       <c r="K236" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L236" s="3" t="s">
         <v>22</v>
@@ -16456,7 +16451,7 @@
         <v>0</v>
       </c>
       <c r="K237" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L237" s="3" t="s">
         <v>22</v>
@@ -16519,7 +16514,7 @@
         <v>50</v>
       </c>
       <c r="K238" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L238" s="3" t="s">
         <v>22</v>
@@ -16582,7 +16577,7 @@
         <v>20</v>
       </c>
       <c r="K239" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L239" s="3" t="s">
         <v>22</v>
@@ -16645,7 +16640,7 @@
         <v>1</v>
       </c>
       <c r="K240" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L240" s="3" t="s">
         <v>22</v>
@@ -16708,7 +16703,7 @@
         <v>20</v>
       </c>
       <c r="K241" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="L241" s="3" t="s">
         <v>22</v>
@@ -16771,7 +16766,7 @@
         <v>5</v>
       </c>
       <c r="K242" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L242" s="3" t="s">
         <v>46</v>
@@ -16834,7 +16829,7 @@
         <v>20</v>
       </c>
       <c r="K243" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L243" s="3" t="s">
         <v>22</v>
@@ -16897,7 +16892,7 @@
         <v>50</v>
       </c>
       <c r="K244" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L244" s="3" t="s">
         <v>22</v>
@@ -16960,7 +16955,7 @@
         <v>20</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="L245" s="3" t="s">
         <v>22</v>
@@ -17023,7 +17018,7 @@
         <v>1</v>
       </c>
       <c r="K246" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L246" s="3" t="s">
         <v>22</v>
@@ -17086,7 +17081,7 @@
         <v>0</v>
       </c>
       <c r="K247" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L247" s="3" t="s">
         <v>22</v>
@@ -17149,7 +17144,7 @@
         <v>0</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L248" s="3" t="s">
         <v>22</v>
@@ -17212,7 +17207,7 @@
         <v>20</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L249" s="3" t="s">
         <v>22</v>
@@ -17275,7 +17270,7 @@
         <v>0</v>
       </c>
       <c r="K250" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L250" s="3" t="s">
         <v>22</v>
@@ -17338,7 +17333,7 @@
         <v>10</v>
       </c>
       <c r="K251" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="L251" s="3" t="s">
         <v>22</v>
@@ -17401,7 +17396,7 @@
         <v>1</v>
       </c>
       <c r="K252" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L252" s="3" t="s">
         <v>22</v>
@@ -17464,7 +17459,7 @@
         <v>0</v>
       </c>
       <c r="K253" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L253" s="3" t="s">
         <v>22</v>
@@ -17527,7 +17522,7 @@
         <v>0</v>
       </c>
       <c r="K254" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L254" s="3" t="s">
         <v>22</v>
@@ -17590,7 +17585,7 @@
         <v>0</v>
       </c>
       <c r="K255" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L255" s="3" t="s">
         <v>22</v>
@@ -17653,7 +17648,7 @@
         <v>0</v>
       </c>
       <c r="K256" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L256" s="3" t="s">
         <v>22</v>
@@ -17716,7 +17711,7 @@
         <v>20</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L257" s="3" t="s">
         <v>22</v>
@@ -17779,7 +17774,7 @@
         <v>0</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L258" s="3" t="s">
         <v>22</v>
@@ -17842,7 +17837,7 @@
         <v>50</v>
       </c>
       <c r="K259" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L259" s="3" t="s">
         <v>22</v>
@@ -17905,7 +17900,7 @@
         <v>5</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L260" s="3" t="s">
         <v>22</v>
@@ -17968,7 +17963,7 @@
         <v>50</v>
       </c>
       <c r="K261" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L261" s="3" t="s">
         <v>22</v>
@@ -18031,7 +18026,7 @@
         <v>5</v>
       </c>
       <c r="K262" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L262" s="3" t="s">
         <v>22</v>
@@ -18094,7 +18089,7 @@
         <v>0</v>
       </c>
       <c r="K263" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L263" s="3" t="s">
         <v>22</v>
@@ -18157,7 +18152,7 @@
         <v>50</v>
       </c>
       <c r="K264" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L264" s="3" t="s">
         <v>22</v>
@@ -18220,7 +18215,7 @@
         <v>50</v>
       </c>
       <c r="K265" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L265" s="3" t="s">
         <v>22</v>
@@ -18283,7 +18278,7 @@
         <v>0</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L266" s="3" t="s">
         <v>22</v>
@@ -18346,7 +18341,7 @@
         <v>1</v>
       </c>
       <c r="K267" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L267" s="3" t="s">
         <v>22</v>
@@ -18409,7 +18404,7 @@
         <v>10</v>
       </c>
       <c r="K268" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L268" s="3" t="s">
         <v>22</v>
@@ -18472,7 +18467,7 @@
         <v>50</v>
       </c>
       <c r="K269" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L269" s="3" t="s">
         <v>22</v>
@@ -18535,7 +18530,7 @@
         <v>20</v>
       </c>
       <c r="K270" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L270" s="3" t="s">
         <v>22</v>
@@ -18598,7 +18593,7 @@
         <v>20</v>
       </c>
       <c r="K271" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L271" s="3" t="s">
         <v>22</v>
@@ -18661,7 +18656,7 @@
         <v>0</v>
       </c>
       <c r="K272" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L272" s="3" t="s">
         <v>22</v>
@@ -18724,7 +18719,7 @@
         <v>1</v>
       </c>
       <c r="K273" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L273" s="3" t="s">
         <v>22</v>
@@ -18787,7 +18782,7 @@
         <v>20</v>
       </c>
       <c r="K274" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L274" s="3" t="s">
         <v>22</v>
@@ -18850,7 +18845,7 @@
         <v>10</v>
       </c>
       <c r="K275" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L275" s="3" t="s">
         <v>22</v>
@@ -18913,7 +18908,7 @@
         <v>5</v>
       </c>
       <c r="K276" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L276" s="3" t="s">
         <v>22</v>
@@ -18976,7 +18971,7 @@
         <v>5</v>
       </c>
       <c r="K277" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="L277" s="3" t="s">
         <v>22</v>
@@ -19033,13 +19028,13 @@
         <v>19</v>
       </c>
       <c r="I278" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J278" s="3">
         <v>20</v>
       </c>
       <c r="K278" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L278" s="3" t="s">
         <v>22</v>
@@ -19096,13 +19091,13 @@
         <v>19</v>
       </c>
       <c r="I279" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J279" s="3">
         <v>10</v>
       </c>
       <c r="K279" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L279" s="3" t="s">
         <v>22</v>
@@ -19159,13 +19154,13 @@
         <v>19</v>
       </c>
       <c r="I280" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J280" s="3">
         <v>5</v>
       </c>
       <c r="K280" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L280" s="3" t="s">
         <v>22</v>
@@ -19222,13 +19217,13 @@
         <v>19</v>
       </c>
       <c r="I281" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J281" s="3">
         <v>0</v>
       </c>
       <c r="K281" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L281" s="3" t="s">
         <v>22</v>
@@ -19285,13 +19280,13 @@
         <v>19</v>
       </c>
       <c r="I282" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J282" s="3">
         <v>5</v>
       </c>
       <c r="K282" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L282" s="3" t="s">
         <v>22</v>
@@ -19348,13 +19343,13 @@
         <v>19</v>
       </c>
       <c r="I283" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J283" s="3">
         <v>1</v>
       </c>
       <c r="K283" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L283" s="3" t="s">
         <v>22</v>
@@ -19411,13 +19406,13 @@
         <v>19</v>
       </c>
       <c r="I284" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J284" s="3">
         <v>20</v>
       </c>
       <c r="K284" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L284" s="3" t="s">
         <v>22</v>
@@ -19474,13 +19469,13 @@
         <v>19</v>
       </c>
       <c r="I285" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J285" s="3">
         <v>10</v>
       </c>
       <c r="K285" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L285" s="3" t="s">
         <v>22</v>
@@ -19537,13 +19532,13 @@
         <v>19</v>
       </c>
       <c r="I286" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J286" s="3">
         <v>10</v>
       </c>
       <c r="K286" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L286" s="3" t="s">
         <v>22</v>
@@ -19600,13 +19595,13 @@
         <v>19</v>
       </c>
       <c r="I287" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J287" s="3">
         <v>10</v>
       </c>
       <c r="K287" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L287" s="3" t="s">
         <v>22</v>
@@ -19663,13 +19658,13 @@
         <v>19</v>
       </c>
       <c r="I288" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J288" s="3">
         <v>1</v>
       </c>
       <c r="K288" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L288" s="3" t="s">
         <v>22</v>
@@ -19726,13 +19721,13 @@
         <v>19</v>
       </c>
       <c r="I289" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J289" s="3">
         <v>10</v>
       </c>
       <c r="K289" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L289" s="3" t="s">
         <v>22</v>
@@ -19789,13 +19784,13 @@
         <v>19</v>
       </c>
       <c r="I290" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J290" s="3">
         <v>5</v>
       </c>
       <c r="K290" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="L290" s="3" t="s">
         <v>22</v>
@@ -19852,13 +19847,13 @@
         <v>19</v>
       </c>
       <c r="I291" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J291" s="3">
         <v>50</v>
       </c>
       <c r="K291" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="L291" s="3" t="s">
         <v>22</v>
@@ -19915,13 +19910,13 @@
         <v>19</v>
       </c>
       <c r="I292" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J292" s="3">
         <v>50</v>
       </c>
       <c r="K292" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L292" s="3" t="s">
         <v>22</v>
@@ -19978,13 +19973,13 @@
         <v>19</v>
       </c>
       <c r="I293" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J293" s="3">
         <v>5</v>
       </c>
       <c r="K293" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L293" s="3" t="s">
         <v>22</v>
@@ -20041,13 +20036,13 @@
         <v>19</v>
       </c>
       <c r="I294" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J294" s="3">
         <v>0</v>
       </c>
       <c r="K294" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L294" s="3" t="s">
         <v>22</v>
@@ -20104,13 +20099,13 @@
         <v>19</v>
       </c>
       <c r="I295" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J295" s="3">
         <v>20</v>
       </c>
       <c r="K295" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L295" s="3" t="s">
         <v>22</v>
@@ -20167,13 +20162,13 @@
         <v>19</v>
       </c>
       <c r="I296" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J296" s="3">
         <v>1</v>
       </c>
       <c r="K296" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L296" s="3" t="s">
         <v>22</v>
@@ -20230,13 +20225,13 @@
         <v>19</v>
       </c>
       <c r="I297" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J297" s="3">
         <v>20</v>
       </c>
       <c r="K297" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L297" s="3" t="s">
         <v>22</v>
@@ -20293,13 +20288,13 @@
         <v>19</v>
       </c>
       <c r="I298" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J298" s="3">
         <v>0</v>
       </c>
       <c r="K298" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L298" s="3" t="s">
         <v>22</v>
@@ -20356,13 +20351,13 @@
         <v>19</v>
       </c>
       <c r="I299" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J299" s="3">
         <v>50</v>
       </c>
       <c r="K299" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L299" s="3" t="s">
         <v>22</v>
@@ -20419,13 +20414,13 @@
         <v>19</v>
       </c>
       <c r="I300" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J300" s="3">
         <v>0</v>
       </c>
       <c r="K300" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L300" s="3" t="s">
         <v>22</v>
@@ -20482,13 +20477,13 @@
         <v>19</v>
       </c>
       <c r="I301" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J301" s="3">
         <v>50</v>
       </c>
       <c r="K301" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L301" s="3" t="s">
         <v>22</v>

</xml_diff>